<commit_message>
Updated temporary system data and tests
</commit_message>
<xml_diff>
--- a/data_tests/generalConfig_testResults.xlsx
+++ b/data_tests/generalConfig_testResults.xlsx
@@ -810,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -842,10 +842,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E3" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -874,10 +874,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -906,10 +906,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -938,10 +938,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1258,10 +1258,10 @@
         <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1322,10 +1322,10 @@
         <v>29</v>
       </c>
       <c r="D18" t="n">
-        <v>29596</v>
+        <v>34006</v>
       </c>
       <c r="E18" t="n">
-        <v>29596</v>
+        <v>34006</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1482,10 +1482,10 @@
         <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>23952</v>
+        <v>24154</v>
       </c>
       <c r="E23" t="n">
-        <v>23952</v>
+        <v>24154</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1627,10 +1627,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1659,10 +1659,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E3" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1691,10 +1691,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1723,10 +1723,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1755,10 +1755,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2075,10 +2075,10 @@
         <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2139,10 +2139,10 @@
         <v>29</v>
       </c>
       <c r="D18" t="n">
-        <v>29596</v>
+        <v>34006</v>
       </c>
       <c r="E18" t="n">
-        <v>29596</v>
+        <v>34006</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -2171,10 +2171,10 @@
         <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>23952</v>
+        <v>24154</v>
       </c>
       <c r="E19" t="n">
-        <v>23952</v>
+        <v>24154</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2267,10 +2267,10 @@
         <v>8</v>
       </c>
       <c r="D22" t="n">
-        <v>217762</v>
+        <v>218344</v>
       </c>
       <c r="E22" t="n">
-        <v>217762</v>
+        <v>218344</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>

</xml_diff>